<commit_message>
aggiustati i file json
</commit_message>
<xml_diff>
--- a/ValutazioneAnnotazioni copia.xlsx
+++ b/ValutazioneAnnotazioni copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiacastiello/Desktop/tesi/code/PreparazioneDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA56E6A-DFCE-8042-90FB-92ECBE3F138A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398311F9-FB96-3948-A70A-6781B3122832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17340" yWindow="940" windowWidth="17060" windowHeight="19560" xr2:uid="{DF822683-9B7D-BD4E-8ECB-3A3E701B4801}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>punteggio</t>
   </si>
@@ -137,10 +137,10 @@
     <t>id19;id26</t>
   </si>
   <si>
-    <t>id17;id2</t>
-  </si>
-  <si>
     <t>id19;id22</t>
+  </si>
+  <si>
+    <t>id17;id20</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,6 +566,9 @@
       <c r="B4">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -593,6 +596,9 @@
       <c r="B7">
         <v>3</v>
       </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -708,7 +714,7 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -766,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -793,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiustati gli errori sull'unione dei file json
</commit_message>
<xml_diff>
--- a/ValutazioneAnnotazioni copia.xlsx
+++ b/ValutazioneAnnotazioni copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiacastiello/Desktop/tesi/code/PreparazioneDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398311F9-FB96-3948-A70A-6781B3122832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598D9B96-1039-B446-8284-7D775D010AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17340" yWindow="940" windowWidth="17060" windowHeight="19560" xr2:uid="{DF822683-9B7D-BD4E-8ECB-3A3E701B4801}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>punteggio</t>
   </si>
@@ -122,25 +122,22 @@
     <t>id25</t>
   </si>
   <si>
-    <t>id26</t>
-  </si>
-  <si>
-    <t>id20; id23</t>
-  </si>
-  <si>
-    <t>id22;id26</t>
-  </si>
-  <si>
-    <t>id17;id23</t>
-  </si>
-  <si>
-    <t>id19;id26</t>
-  </si>
-  <si>
-    <t>id19;id22</t>
-  </si>
-  <si>
-    <t>id17;id20</t>
+    <t>id18;id21</t>
+  </si>
+  <si>
+    <t>id16;id19</t>
+  </si>
+  <si>
+    <t>id18;id25</t>
+  </si>
+  <si>
+    <t>id16;id22</t>
+  </si>
+  <si>
+    <t>id21;id25</t>
+  </si>
+  <si>
+    <t>id19; id22</t>
   </si>
 </sst>
 </file>
@@ -518,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2073A893-7ED7-7C44-9169-48B682ECA820}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -648,9 +645,6 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -667,16 +661,16 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -684,10 +678,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -695,7 +686,10 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -706,7 +700,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -714,10 +708,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -728,7 +722,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -736,10 +730,10 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -750,7 +744,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -758,10 +752,10 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -771,9 +765,6 @@
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -790,16 +781,8 @@
       <c r="B26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C26" t="s">
         <v>28</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>